<commit_message>
updating peprocessing for feature engineering individual areas
- made some adjustments to the preprocessing step for the feature engineering for individual areas using the hierarchical cluster method
-this way the same work procedure is followed
</commit_message>
<xml_diff>
--- a/_CLUSTER/groups_time_area/interpolation/combined_Fe/comparison_areas.xlsx
+++ b/_CLUSTER/groups_time_area/interpolation/combined_Fe/comparison_areas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sebastian\Desktop\python_map\New\Vistelius_1995_OCR\_CLUSTER\groups_time_area\interpolation\combined_Fe\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1B18D40-3E9C-4546-BF96-EF00DF185631}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8F1C14E-A3D5-431C-9FDB-95E84C7F6BFC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DA85E2DB-5D01-4214-9D4D-3B0C9A6B185E}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="8">
   <si>
     <t>Area1</t>
   </si>
@@ -85,12 +85,18 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -120,12 +126,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -440,23 +447,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECBA17AE-F5B6-4BAA-AB65-7E73791AF0D9}">
-  <dimension ref="A1:S10"/>
+  <dimension ref="A1:S26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>6</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -464,229 +468,329 @@
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
       <c r="I1" t="s">
         <v>3</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
       <c r="M1" t="s">
         <v>4</v>
       </c>
       <c r="N1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="O1" t="s">
-        <v>6</v>
-      </c>
       <c r="Q1" t="s">
         <v>5</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="S1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
         <v>50491</v>
       </c>
-      <c r="C2">
-        <f>B2/$B$4*100</f>
-        <v>91.1176077815675</v>
-      </c>
       <c r="E2" s="1">
         <v>0</v>
       </c>
       <c r="F2">
         <v>29079</v>
       </c>
-      <c r="G2">
-        <f>F2/$F$4*100</f>
-        <v>61.818916218457019</v>
-      </c>
       <c r="I2" s="1">
         <v>0</v>
       </c>
       <c r="J2">
         <v>40830</v>
       </c>
-      <c r="K2">
-        <f>J2/$J$4*100</f>
-        <v>74.979340740060593</v>
-      </c>
       <c r="M2" s="1">
         <v>0</v>
       </c>
       <c r="N2">
         <v>22925</v>
       </c>
-      <c r="O2">
-        <f>N2/$N$4*100</f>
-        <v>38.543015181828885</v>
-      </c>
       <c r="Q2" s="1">
         <v>0</v>
       </c>
       <c r="R2">
         <v>53363</v>
       </c>
-      <c r="S2">
-        <f>R2/$R$4*100</f>
-        <v>88.62960686940491</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
         <v>4922</v>
       </c>
-      <c r="C3">
-        <f t="shared" ref="C3:C4" si="0">B3/$B$4*100</f>
-        <v>8.8823922184324964</v>
-      </c>
       <c r="E3" s="1">
         <v>1</v>
       </c>
       <c r="F3">
         <v>17960</v>
       </c>
-      <c r="G3">
-        <f t="shared" ref="G3:G4" si="1">F3/$F$4*100</f>
-        <v>38.181083781542974</v>
-      </c>
       <c r="I3" s="1">
         <v>1</v>
       </c>
       <c r="J3">
         <v>13625</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K4" si="2">J3/$J$4*100</f>
-        <v>25.0206592599394</v>
-      </c>
       <c r="M3" s="1">
         <v>1</v>
       </c>
       <c r="N3">
         <v>36554</v>
       </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O4" si="3">N3/$N$4*100</f>
-        <v>61.456984818171122</v>
-      </c>
       <c r="Q3" s="1">
         <v>1</v>
       </c>
       <c r="R3">
         <v>6846</v>
       </c>
-      <c r="S3">
-        <f t="shared" ref="S3:S4" si="4">R3/$R$4*100</f>
+    </row>
+    <row r="15" spans="1:18" s="3" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" t="s">
+        <v>6</v>
+      </c>
+      <c r="I17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="K17" t="s">
+        <v>6</v>
+      </c>
+      <c r="M17" t="s">
+        <v>4</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="O17" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>5</v>
+      </c>
+      <c r="R17" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>50491</v>
+      </c>
+      <c r="C18">
+        <f>B18/$B$20*100</f>
+        <v>91.1176077815675</v>
+      </c>
+      <c r="E18" s="1">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>29079</v>
+      </c>
+      <c r="G18">
+        <f>F18/$F$20*100</f>
+        <v>61.818916218457019</v>
+      </c>
+      <c r="I18" s="1">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>40830</v>
+      </c>
+      <c r="K18">
+        <f>J18/$J$20*100</f>
+        <v>74.979340740060593</v>
+      </c>
+      <c r="M18" s="1">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>22925</v>
+      </c>
+      <c r="O18">
+        <f>N18/$N$20*100</f>
+        <v>38.543015181828885</v>
+      </c>
+      <c r="Q18" s="1">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>53363</v>
+      </c>
+      <c r="S18">
+        <f>R18/$R$20*100</f>
+        <v>88.62960686940491</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>1</v>
+      </c>
+      <c r="B19">
+        <v>4922</v>
+      </c>
+      <c r="C19">
+        <f t="shared" ref="C19:C20" si="0">B19/$B$20*100</f>
+        <v>8.8823922184324964</v>
+      </c>
+      <c r="E19" s="1">
+        <v>1</v>
+      </c>
+      <c r="F19">
+        <v>17960</v>
+      </c>
+      <c r="G19">
+        <f t="shared" ref="G19:G20" si="1">F19/$F$20*100</f>
+        <v>38.181083781542974</v>
+      </c>
+      <c r="I19" s="1">
+        <v>1</v>
+      </c>
+      <c r="J19">
+        <v>13625</v>
+      </c>
+      <c r="K19">
+        <f t="shared" ref="K19:K20" si="2">J19/$J$20*100</f>
+        <v>25.0206592599394</v>
+      </c>
+      <c r="M19" s="1">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>36554</v>
+      </c>
+      <c r="O19">
+        <f t="shared" ref="O19:O20" si="3">N19/$N$20*100</f>
+        <v>61.456984818171122</v>
+      </c>
+      <c r="Q19" s="1">
+        <v>1</v>
+      </c>
+      <c r="R19">
+        <v>6846</v>
+      </c>
+      <c r="S19">
+        <f t="shared" ref="S19:S20" si="4">R19/$R$20*100</f>
         <v>11.370393130595094</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B4" s="2">
-        <f>SUM(B2:B3)</f>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B20" s="2">
+        <f>SUM(B18:B19)</f>
         <v>55413</v>
       </c>
-      <c r="C4">
+      <c r="C20">
         <f t="shared" si="0"/>
         <v>100</v>
       </c>
-      <c r="F4" s="2">
-        <f>SUM(F2:F3)</f>
+      <c r="F20" s="2">
+        <f>SUM(F18:F19)</f>
         <v>47039</v>
       </c>
-      <c r="G4">
+      <c r="G20">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-      <c r="J4" s="2">
-        <f>SUM(J2:J3)</f>
+      <c r="J20" s="2">
+        <f>SUM(J18:J19)</f>
         <v>54455</v>
       </c>
-      <c r="K4">
+      <c r="K20">
         <f t="shared" si="2"/>
         <v>100</v>
       </c>
-      <c r="N4" s="2">
-        <f>SUM(N2:N3)</f>
+      <c r="N20" s="2">
+        <f>SUM(N18:N19)</f>
         <v>59479</v>
       </c>
-      <c r="O4">
+      <c r="O20">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="R4" s="2">
-        <f>SUM(R2:R3)</f>
+      <c r="R20" s="2">
+        <f>SUM(R18:R19)</f>
         <v>60209</v>
       </c>
-      <c r="S4">
+      <c r="S20">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B5" s="2"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="B23" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>1</v>
-      </c>
-      <c r="B8">
-        <f>B2+F2+J2+N2+R2</f>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <f>B18+F18+J18+N18+R18</f>
         <v>196688</v>
       </c>
-      <c r="C8">
-        <f>B8/$B$10*100</f>
+      <c r="C24">
+        <f>B24/$B$26*100</f>
         <v>71.110468374337927</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <f t="shared" ref="B9:B10" si="5">B3+F3+J3+N3+R3</f>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <f t="shared" ref="B25:B26" si="5">B19+F19+J19+N19+R19</f>
         <v>79907</v>
       </c>
-      <c r="C9">
-        <f t="shared" ref="C9:C10" si="6">B9/$B$10*100</f>
+      <c r="C25">
+        <f t="shared" ref="C25:C26" si="6">B25/$B$26*100</f>
         <v>28.88953162566207</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="B10">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B26">
         <f t="shared" si="5"/>
         <v>276595</v>
       </c>
-      <c r="C10">
+      <c r="C26">
         <f t="shared" si="6"/>
         <v>100</v>
       </c>

</xml_diff>